<commit_message>
playing with the xlsx library
</commit_message>
<xml_diff>
--- a/UD_Test.xlsx
+++ b/UD_Test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9b150c228a8ec7fd/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9b150c228a8ec7fd/Documents/github/TW/TW-Calculators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AD71655-AFE1-4F6F-A3AA-1B3185552D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{9AD71655-AFE1-4F6F-A3AA-1B3185552D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{630A53B7-4C9C-4813-8CBC-4524D1B26E45}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{138D0947-FEEF-4F14-88FC-FC6CA08A5741}"/>
   </bookViews>
@@ -156,12 +156,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -176,9 +182,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -521,7 +530,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -550,7 +559,7 @@
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">

</xml_diff>